<commit_message>
initial database wide monte carlo
</commit_message>
<xml_diff>
--- a/Calculation time and size.xlsx
+++ b/Calculation time and size.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="38">
   <si>
     <t>Storage size in HDF5 [MB]</t>
   </si>
@@ -106,6 +106,33 @@
   </si>
   <si>
     <t>all</t>
+  </si>
+  <si>
+    <t>Matrice G</t>
+  </si>
+  <si>
+    <t>Matrix G</t>
+  </si>
+  <si>
+    <t>Matrix B</t>
+  </si>
+  <si>
+    <t>Vector s</t>
+  </si>
+  <si>
+    <t>Matrix B and vector s</t>
+  </si>
+  <si>
+    <t>Matrix A</t>
+  </si>
+  <si>
+    <t>Benoit Foret</t>
+  </si>
+  <si>
+    <t>4TB</t>
+  </si>
+  <si>
+    <t>Direct object size</t>
   </si>
 </sst>
 </file>
@@ -172,10 +199,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:K22"/>
+  <dimension ref="A3:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -470,7 +497,7 @@
     <col min="5" max="5" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>20</v>
       </c>
@@ -478,7 +505,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -495,7 +522,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -510,7 +537,7 @@
       </c>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -525,7 +552,7 @@
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -540,7 +567,7 @@
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -555,7 +582,7 @@
       </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -573,7 +600,7 @@
       </c>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -588,7 +615,7 @@
       </c>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -603,7 +630,7 @@
       </c>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -618,7 +645,7 @@
       </c>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -635,7 +662,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
         <v>28</v>
       </c>
@@ -643,231 +670,367 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" t="s">
-        <v>23</v>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B15" s="1"/>
+      <c r="C15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16">
+        <v>2.5</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" t="s">
-        <v>0</v>
-      </c>
-      <c r="D17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E17" t="s">
-        <v>18</v>
-      </c>
-      <c r="F17" t="s">
-        <v>22</v>
-      </c>
-      <c r="G17" t="s">
-        <v>17</v>
-      </c>
-      <c r="H17" t="s">
-        <v>18</v>
-      </c>
-      <c r="I17" t="s">
-        <v>25</v>
-      </c>
-      <c r="J17" t="s">
-        <v>24</v>
-      </c>
-      <c r="K17" t="s">
-        <v>26</v>
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17">
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
+        <v>14</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="C18">
-        <f>$B18*SUMIF($A$5:$A$13,$A18,$C$5:$C$13)</f>
-        <v>0.23697599999999999</v>
-      </c>
-      <c r="D18">
-        <f>C18/1000</f>
-        <v>2.3697599999999999E-4</v>
-      </c>
-      <c r="E18" s="2">
-        <f>D18/1000</f>
-        <v>2.3697599999999999E-7</v>
-      </c>
-      <c r="F18">
-        <f>$B18*SUMIF($A$5:$A$13,$A18,$D$5:$D$13)</f>
-        <v>8.326900000000001E-2</v>
-      </c>
-      <c r="G18">
-        <f>F18/1000</f>
-        <v>8.3269000000000005E-5</v>
-      </c>
-      <c r="H18" s="2">
-        <f>G18/1000</f>
-        <v>8.3269000000000003E-8</v>
+        <v>0.109</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B21" s="1"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" t="s">
+        <v>22</v>
+      </c>
+      <c r="G24" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24" t="s">
+        <v>18</v>
+      </c>
+      <c r="I24" t="s">
+        <v>25</v>
+      </c>
+      <c r="J24" t="s">
+        <v>24</v>
+      </c>
+      <c r="K24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <f>$B25*SUMIF($A$5:$A$13,$A25,$C$5:$C$13)</f>
+        <v>0.23697599999999999</v>
+      </c>
+      <c r="D25">
+        <f>C25/1000</f>
+        <v>2.3697599999999999E-4</v>
+      </c>
+      <c r="E25" s="2">
+        <f>D25/1000</f>
+        <v>2.3697599999999999E-7</v>
+      </c>
+      <c r="F25">
+        <f>$B25*SUMIF($A$5:$A$13,$A25,$D$5:$D$13)</f>
+        <v>8.326900000000001E-2</v>
+      </c>
+      <c r="G25">
+        <f>F25/1000</f>
+        <v>8.3269000000000005E-5</v>
+      </c>
+      <c r="H25" s="2">
+        <f>G25/1000</f>
+        <v>8.3269000000000003E-8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>12</v>
       </c>
-      <c r="B19">
+      <c r="B26">
         <v>13831</v>
       </c>
-      <c r="C19">
-        <f t="shared" ref="C19:C21" si="0">$B19*SUMIF($A$5:$A$13,$A19,$C$5:$C$13)</f>
+      <c r="C26">
+        <f t="shared" ref="C26:C28" si="0">$B26*SUMIF($A$5:$A$13,$A26,$C$5:$C$13)</f>
         <v>298049.25348399999</v>
       </c>
-      <c r="D19">
-        <f t="shared" ref="D19:E22" si="1">C19/1000</f>
+      <c r="D26">
+        <f t="shared" ref="D26:E29" si="1">C26/1000</f>
         <v>298.04925348399996</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E26" s="2">
         <f t="shared" si="1"/>
         <v>0.29804925348399997</v>
       </c>
-      <c r="F19">
-        <f t="shared" ref="F19:F21" si="2">$B19*SUMIF($A$5:$A$13,$A19,$D$5:$D$13)</f>
+      <c r="F26">
+        <f t="shared" ref="F26:F28" si="2">$B26*SUMIF($A$5:$A$13,$A26,$D$5:$D$13)</f>
         <v>86295.578496999995</v>
       </c>
-      <c r="G19">
-        <f t="shared" ref="G19:G22" si="3">F19/1000</f>
+      <c r="G26">
+        <f t="shared" ref="G26:G29" si="3">F26/1000</f>
         <v>86.295578496999994</v>
       </c>
-      <c r="H19" s="2">
-        <f t="shared" ref="H19:I22" si="4">G19/1000</f>
+      <c r="H26" s="2">
+        <f t="shared" ref="H26:H29" si="4">G26/1000</f>
         <v>8.6295578496999994E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>13</v>
       </c>
-      <c r="B20">
+      <c r="B27">
         <v>1000</v>
       </c>
-      <c r="C20">
+      <c r="C27">
         <f t="shared" si="0"/>
         <v>4009.1839999999993</v>
       </c>
-      <c r="D20">
+      <c r="D27">
         <f t="shared" si="1"/>
         <v>4.0091839999999994</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E27" s="2">
         <f t="shared" si="1"/>
         <v>4.0091839999999998E-3</v>
       </c>
-      <c r="F20">
+      <c r="F27">
         <f t="shared" si="2"/>
         <v>3032.5459999999998</v>
       </c>
-      <c r="G20">
+      <c r="G27">
         <f t="shared" si="3"/>
         <v>3.032546</v>
       </c>
-      <c r="H20" s="2">
+      <c r="H27" s="2">
         <f t="shared" si="4"/>
         <v>3.0325460000000001E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>14</v>
       </c>
-      <c r="B21">
-        <f>B19*B20</f>
+      <c r="B28">
+        <f>B26*B27</f>
         <v>13831000</v>
       </c>
-      <c r="C21">
+      <c r="C28">
         <f t="shared" si="0"/>
         <v>83991845.643999994</v>
       </c>
-      <c r="D21">
+      <c r="D28">
         <f t="shared" si="1"/>
         <v>83991.845644000001</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E28" s="2">
         <f t="shared" si="1"/>
         <v>83.991845643999994</v>
       </c>
-      <c r="F21">
+      <c r="F28">
         <f t="shared" si="2"/>
         <v>36636922.068999998</v>
       </c>
-      <c r="G21">
+      <c r="G28">
         <f t="shared" si="3"/>
         <v>36636.922069</v>
       </c>
-      <c r="H21" s="2">
+      <c r="H28" s="2">
         <f t="shared" si="4"/>
         <v>36.636922069000001</v>
       </c>
-      <c r="I21">
-        <f>$B21*SUMIF($A$5:$A$13,$A21,$E$5:$E$13)</f>
+      <c r="I28">
+        <f>$B28*SUMIF($A$5:$A$13,$A28,$E$5:$E$13)</f>
         <v>1383100</v>
       </c>
-      <c r="J21" s="7">
-        <f>I21/3600</f>
+      <c r="J28" s="6">
+        <f>I28/3600</f>
         <v>384.19444444444446</v>
       </c>
-      <c r="K21" s="7">
-        <f>J21/24</f>
+      <c r="K28" s="6">
+        <f>J28/24</f>
         <v>16.008101851851851</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4">
-        <f>SUM(C18:C21)</f>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4">
+        <f>SUM(C25:C28)</f>
         <v>84293904.318459988</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D29" s="4">
         <f t="shared" si="1"/>
         <v>84293.904318459987</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E29" s="5">
         <f t="shared" si="1"/>
         <v>84.293904318459994</v>
       </c>
-      <c r="F22" s="4">
-        <f>SUM(F18:F21)</f>
+      <c r="F29" s="4">
+        <f>SUM(F25:F28)</f>
         <v>36726250.276765995</v>
       </c>
-      <c r="G22" s="4">
+      <c r="G29" s="4">
         <f t="shared" si="3"/>
         <v>36726.250276765997</v>
       </c>
-      <c r="H22" s="5">
+      <c r="H29" s="5">
         <f t="shared" si="4"/>
         <v>36.726250276765995</v>
       </c>
     </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H30" s="2"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32">
+        <f>B28*C16</f>
+        <v>34577500</v>
+      </c>
+      <c r="D32">
+        <f t="shared" ref="D32" si="5">C32/1000</f>
+        <v>34577.5</v>
+      </c>
+      <c r="E32" s="2">
+        <f t="shared" ref="E32" si="6">D32/1000</f>
+        <v>34.577500000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35">
+        <f>B27</f>
+        <v>1000</v>
+      </c>
+      <c r="C35">
+        <f>B35*(C17+C19)</f>
+        <v>7500</v>
+      </c>
+      <c r="D35">
+        <f t="shared" ref="D35:D36" si="7">C35/1000</f>
+        <v>7.5</v>
+      </c>
+      <c r="E35" s="2">
+        <f t="shared" ref="E35:E36" si="8">D35/1000</f>
+        <v>7.4999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36">
+        <f>B28</f>
+        <v>13831000</v>
+      </c>
+      <c r="C36">
+        <f>B36*C18</f>
+        <v>1507579</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="7"/>
+        <v>1507.579</v>
+      </c>
+      <c r="E36" s="2">
+        <f t="shared" si="8"/>
+        <v>1.507579</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="F23:H23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Test of Dep MC with HDF5
</commit_message>
<xml_diff>
--- a/Calculation time and size.xlsx
+++ b/Calculation time and size.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="For dependant MC" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -18,8 +19,66 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Auteur</author>
+  </authors>
+  <commentList>
+    <comment ref="F11" authorId="0" shapeId="0" xr:uid="{DB0AE222-00F3-4202-B9BE-89B338D23222}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Juste the first activity takes 0.5 sec </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F12" authorId="0" shapeId="0" xr:uid="{ADCC4501-0FAA-4B31-8FA7-F49CA2BF5F32}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Time for A and B --&gt; max of iteration tested</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="42">
   <si>
     <t>Storage size in HDF5 [MB]</t>
   </si>
@@ -133,13 +192,25 @@
   </si>
   <si>
     <t>Direct object size</t>
+  </si>
+  <si>
+    <t>supply_array</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Without multiprocessing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,6 +239,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -485,7 +569,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -1035,4 +1119,559 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5E8E4FE-D9C4-4A09-8B44-2D595489B0E8}">
+  <dimension ref="A3:N37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" customWidth="1"/>
+    <col min="3" max="3" width="23.44140625" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <f>490424/1000000</f>
+        <v>0.49042400000000003</v>
+      </c>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11">
+        <f>43700/1000000</f>
+        <v>4.3700000000000003E-2</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="G11">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <f>349175/1000000</f>
+        <v>0.34917500000000001</v>
+      </c>
+      <c r="F12">
+        <v>0.4</v>
+      </c>
+      <c r="G12">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="1"/>
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" t="s">
+        <v>23</v>
+      </c>
+      <c r="L22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" t="s">
+        <v>22</v>
+      </c>
+      <c r="G23" t="s">
+        <v>17</v>
+      </c>
+      <c r="H23" t="s">
+        <v>18</v>
+      </c>
+      <c r="I23" t="s">
+        <v>25</v>
+      </c>
+      <c r="J23" t="s">
+        <v>24</v>
+      </c>
+      <c r="K23" t="s">
+        <v>26</v>
+      </c>
+      <c r="L23" t="s">
+        <v>25</v>
+      </c>
+      <c r="M23" t="s">
+        <v>24</v>
+      </c>
+      <c r="N23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <f>$B24*SUMIF($A$5:$A$12,$A24,$C$5:$C$12)</f>
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <f>C24/1000</f>
+        <v>0</v>
+      </c>
+      <c r="E24" s="2">
+        <f>D24/1000</f>
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <f>$B24*SUMIF($A$5:$A$12,$A24,$D$5:$D$12)</f>
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <f>F24/1000</f>
+        <v>0</v>
+      </c>
+      <c r="H24" s="2">
+        <f>G24/1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25">
+        <v>13831</v>
+      </c>
+      <c r="C25">
+        <f>$B25*SUMIF($A$5:$A$12,$A25,$C$5:$C$12)</f>
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <f t="shared" ref="D25:E28" si="0">C25/1000</f>
+        <v>0</v>
+      </c>
+      <c r="E25" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <f>$B25*SUMIF($A$5:$A$12,$A25,$D$5:$D$12)</f>
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <f t="shared" ref="G25:H28" si="1">F25/1000</f>
+        <v>0</v>
+      </c>
+      <c r="H25" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26">
+        <v>1000</v>
+      </c>
+      <c r="C26">
+        <f>$B26*SUMIF($A$5:$A$12,$A26,$C$5:$C$12)</f>
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E26" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <f>$B26*SUMIF($A$5:$A$12,$A26,$D$5:$D$12)</f>
+        <v>839.59899999999993</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="1"/>
+        <v>0.83959899999999998</v>
+      </c>
+      <c r="H26" s="2">
+        <f t="shared" si="1"/>
+        <v>8.3959900000000001E-4</v>
+      </c>
+      <c r="L26">
+        <f>$B26*SUMIF($A$5:$A$12,$A26,$F$5:$F$12)</f>
+        <v>400</v>
+      </c>
+      <c r="M26" s="6">
+        <f>L26/3600</f>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="N26" s="6">
+        <f>M26/24</f>
+        <v>4.6296296296296294E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27">
+        <f>B25*B26</f>
+        <v>13831000</v>
+      </c>
+      <c r="C27">
+        <f>$B27*SUMIF($A$5:$A$12,$A27,$C$5:$C$12)</f>
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E27" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <f>$B27*SUMIF($A$5:$A$12,$A27,$D$5:$D$12)</f>
+        <v>604414.70000000007</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="1"/>
+        <v>604.41470000000004</v>
+      </c>
+      <c r="H27" s="2">
+        <f t="shared" si="1"/>
+        <v>0.60441470000000008</v>
+      </c>
+      <c r="I27">
+        <f>$B27*SUMIF($A$5:$A$12,$A27,$E$5:$E$12)</f>
+        <v>0</v>
+      </c>
+      <c r="J27" s="6">
+        <f>I27/3600</f>
+        <v>0</v>
+      </c>
+      <c r="K27" s="6">
+        <f>J27/24</f>
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <f>$B27*SUMIF($A$5:$A$12,$A27,$F$5:$F$12)</f>
+        <v>138310</v>
+      </c>
+      <c r="M27" s="6">
+        <f>L27/3600</f>
+        <v>38.419444444444444</v>
+      </c>
+      <c r="N27" s="6">
+        <f>M27/24</f>
+        <v>1.6008101851851853</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4">
+        <f>SUM(C24:C27)</f>
+        <v>0</v>
+      </c>
+      <c r="D28" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E28" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F28" s="4">
+        <f>SUM(F24:F27)</f>
+        <v>605254.29900000012</v>
+      </c>
+      <c r="G28" s="4">
+        <f t="shared" si="1"/>
+        <v>605.25429900000006</v>
+      </c>
+      <c r="H28" s="5">
+        <f t="shared" si="1"/>
+        <v>0.60525429900000005</v>
+      </c>
+      <c r="L28" s="4">
+        <f>SUM(L24:L27)</f>
+        <v>138710</v>
+      </c>
+      <c r="M28" s="5">
+        <f t="shared" ref="M28:N28" si="2">SUM(M24:M27)</f>
+        <v>38.530555555555559</v>
+      </c>
+      <c r="N28" s="5">
+        <f t="shared" si="2"/>
+        <v>1.6054398148148148</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31">
+        <f>B27*C15</f>
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <f t="shared" ref="D31:E31" si="3">C31/1000</f>
+        <v>0</v>
+      </c>
+      <c r="E31" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34">
+        <f>B26</f>
+        <v>1000</v>
+      </c>
+      <c r="C34">
+        <f>B34*(C16+C18)</f>
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <f t="shared" ref="D34:E35" si="4">C34/1000</f>
+        <v>0</v>
+      </c>
+      <c r="E34" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35">
+        <f>B27</f>
+        <v>13831000</v>
+      </c>
+      <c r="C35">
+        <f>B35*C17</f>
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E35" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="F22:H22"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Monte Carlo LCA calculation script initial
</commit_message>
<xml_diff>
--- a/Calculation time and size.xlsx
+++ b/Calculation time and size.xlsx
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="44">
   <si>
     <t>Storage size in HDF5 [MB]</t>
   </si>
@@ -204,6 +204,12 @@
   </si>
   <si>
     <t>Without multiprocessing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">With </t>
+  </si>
+  <si>
+    <t>processes</t>
   </si>
 </sst>
 </file>
@@ -1123,10 +1129,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5E8E4FE-D9C4-4A09-8B44-2D595489B0E8}">
-  <dimension ref="A3:N37"/>
+  <dimension ref="A3:Q37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="R26" sqref="R26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1203,8 +1209,8 @@
         <v>6</v>
       </c>
       <c r="D8">
-        <f>490424/1000000</f>
-        <v>0.49042400000000003</v>
+        <f>1.7375</f>
+        <v>1.7375</v>
       </c>
       <c r="F8" s="1"/>
     </row>
@@ -1252,11 +1258,11 @@
         <v>10</v>
       </c>
       <c r="D12">
-        <f>349175/1000000</f>
-        <v>0.34917500000000001</v>
+        <f>0.84333</f>
+        <v>0.84333000000000002</v>
       </c>
       <c r="F12">
-        <v>0.4</v>
+        <v>0.35</v>
       </c>
       <c r="G12">
         <v>0.27</v>
@@ -1289,7 +1295,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1297,7 +1303,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -1305,18 +1311,31 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="L21" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O21" t="s">
+        <v>42</v>
+      </c>
+      <c r="P21">
+        <f>$P$20</f>
+        <v>4</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>15</v>
       </c>
@@ -1336,8 +1355,11 @@
       <c r="L22" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>16</v>
       </c>
@@ -1377,8 +1399,17 @@
       <c r="N23" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O23" t="s">
+        <v>25</v>
+      </c>
+      <c r="P23" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>11</v>
       </c>
@@ -1409,8 +1440,20 @@
         <f>G24/1000</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O24">
+        <f>(L24)/($P$20)</f>
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <f>(M24)/($P$20)</f>
+        <v>0</v>
+      </c>
+      <c r="Q24">
+        <f>(N24)/($P$20)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -1441,8 +1484,20 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O25">
+        <f>(L25)/($P$20)</f>
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <f>(M25)/($P$20)</f>
+        <v>0</v>
+      </c>
+      <c r="Q25">
+        <f>(N25)/($P$20)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>13</v>
       </c>
@@ -1463,30 +1518,42 @@
       </c>
       <c r="F26">
         <f>$B26*SUMIF($A$5:$A$12,$A26,$D$5:$D$12)</f>
-        <v>839.59899999999993</v>
+        <v>2580.8300000000004</v>
       </c>
       <c r="G26">
         <f t="shared" si="1"/>
-        <v>0.83959899999999998</v>
+        <v>2.5808300000000002</v>
       </c>
       <c r="H26" s="2">
         <f t="shared" si="1"/>
-        <v>8.3959900000000001E-4</v>
+        <v>2.5808300000000001E-3</v>
       </c>
       <c r="L26">
         <f>$B26*SUMIF($A$5:$A$12,$A26,$F$5:$F$12)</f>
-        <v>400</v>
+        <v>350</v>
       </c>
       <c r="M26" s="6">
         <f>L26/3600</f>
-        <v>0.1111111111111111</v>
+        <v>9.7222222222222224E-2</v>
       </c>
       <c r="N26" s="6">
         <f>M26/24</f>
-        <v>4.6296296296296294E-3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+        <v>4.0509259259259257E-3</v>
+      </c>
+      <c r="O26">
+        <f>(L26)/($P$20)</f>
+        <v>87.5</v>
+      </c>
+      <c r="P26">
+        <f>(M26)/($P$20)</f>
+        <v>2.4305555555555556E-2</v>
+      </c>
+      <c r="Q26">
+        <f>(N26)/($P$20)</f>
+        <v>1.0127314814814814E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -1542,8 +1609,20 @@
         <f>M27/24</f>
         <v>1.6008101851851853</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O27">
+        <f>(L27)/($P$20)</f>
+        <v>34577.5</v>
+      </c>
+      <c r="P27">
+        <f>(M27)/($P$20)</f>
+        <v>9.6048611111111111</v>
+      </c>
+      <c r="Q27">
+        <f>(N27)/($P$20)</f>
+        <v>0.40020254629629631</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>19</v>
       </c>
@@ -1562,38 +1641,50 @@
       </c>
       <c r="F28" s="4">
         <f>SUM(F24:F27)</f>
-        <v>605254.29900000012</v>
+        <v>606995.53</v>
       </c>
       <c r="G28" s="4">
         <f t="shared" si="1"/>
-        <v>605.25429900000006</v>
+        <v>606.99553000000003</v>
       </c>
       <c r="H28" s="5">
         <f t="shared" si="1"/>
-        <v>0.60525429900000005</v>
+        <v>0.60699553000000006</v>
       </c>
       <c r="L28" s="4">
         <f>SUM(L24:L27)</f>
-        <v>138710</v>
+        <v>138660</v>
       </c>
       <c r="M28" s="5">
         <f t="shared" ref="M28:N28" si="2">SUM(M24:M27)</f>
-        <v>38.530555555555559</v>
+        <v>38.516666666666666</v>
       </c>
       <c r="N28" s="5">
         <f t="shared" si="2"/>
-        <v>1.6054398148148148</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+        <v>1.6048611111111111</v>
+      </c>
+      <c r="O28" s="4">
+        <f>SUM(O24:O27)</f>
+        <v>34665</v>
+      </c>
+      <c r="P28" s="5">
+        <f t="shared" ref="P28:Q28" si="3">SUM(P24:P27)</f>
+        <v>9.6291666666666664</v>
+      </c>
+      <c r="Q28" s="5">
+        <f t="shared" si="3"/>
+        <v>0.40121527777777777</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -1602,11 +1693,11 @@
         <v>0</v>
       </c>
       <c r="D31">
-        <f t="shared" ref="D31:E31" si="3">C31/1000</f>
+        <f t="shared" ref="D31:E31" si="4">C31/1000</f>
         <v>0</v>
       </c>
       <c r="E31" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -1628,11 +1719,11 @@
         <v>0</v>
       </c>
       <c r="D34">
-        <f t="shared" ref="D34:E35" si="4">C34/1000</f>
+        <f t="shared" ref="D34:E35" si="5">C34/1000</f>
         <v>0</v>
       </c>
       <c r="E34" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -1649,11 +1740,11 @@
         <v>0</v>
       </c>
       <c r="D35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E35" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finalize LCI and LCA Monte Carlo
</commit_message>
<xml_diff>
--- a/Calculation time and size.xlsx
+++ b/Calculation time and size.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
-    <sheet name="For dependant MC" sheetId="2" r:id="rId2"/>
+    <sheet name="Dependant LCI MC" sheetId="2" r:id="rId2"/>
+    <sheet name="Dependant LCA MC" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -77,8 +78,91 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Auteur</author>
+  </authors>
+  <commentList>
+    <comment ref="D5" authorId="0" shapeId="0" xr:uid="{649FA4CF-E93B-44E5-828B-790509186BBE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+results</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D6" authorId="0" shapeId="0" xr:uid="{DF30E2A0-7499-4942-B952-B68695DDCF35}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+results
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F7" authorId="0" shapeId="0" xr:uid="{98118E98-063D-4DA8-9C75-02C2E573C1BE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+0.004 grand max</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="53">
   <si>
     <t>Storage size in HDF5 [MB]</t>
   </si>
@@ -210,6 +294,33 @@
   </si>
   <si>
     <t>processes</t>
+  </si>
+  <si>
+    <t>Object</t>
+  </si>
+  <si>
+    <t>per iter and act and IC</t>
+  </si>
+  <si>
+    <t>per worker</t>
+  </si>
+  <si>
+    <t>aggregated</t>
+  </si>
+  <si>
+    <t>disaggregated</t>
+  </si>
+  <si>
+    <t>Number of IC</t>
+  </si>
+  <si>
+    <t>For aggregated and disaggregated</t>
+  </si>
+  <si>
+    <t>Disaggregated and aggregated</t>
+  </si>
+  <si>
+    <t>For aggregated</t>
   </si>
 </sst>
 </file>
@@ -1131,8 +1242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5E8E4FE-D9C4-4A09-8B44-2D595489B0E8}">
   <dimension ref="A3:Q37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R26" sqref="R26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1441,15 +1552,15 @@
         <v>0</v>
       </c>
       <c r="O24">
-        <f>(L24)/($P$20)</f>
+        <f t="shared" ref="O24:Q27" si="0">(L24)/($P$20)</f>
         <v>0</v>
       </c>
       <c r="P24">
-        <f>(M24)/($P$20)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q24">
-        <f>(N24)/($P$20)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1465,11 +1576,11 @@
         <v>0</v>
       </c>
       <c r="D25">
-        <f t="shared" ref="D25:E28" si="0">C25/1000</f>
+        <f t="shared" ref="D25:E28" si="1">C25/1000</f>
         <v>0</v>
       </c>
       <c r="E25" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F25">
@@ -1477,23 +1588,23 @@
         <v>0</v>
       </c>
       <c r="G25">
-        <f t="shared" ref="G25:H28" si="1">F25/1000</f>
+        <f t="shared" ref="G25:H28" si="2">F25/1000</f>
         <v>0</v>
       </c>
       <c r="H25" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O25">
-        <f>(L25)/($P$20)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P25">
-        <f>(M25)/($P$20)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q25">
-        <f>(N25)/($P$20)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1509,11 +1620,11 @@
         <v>0</v>
       </c>
       <c r="D26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E26" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F26">
@@ -1521,11 +1632,11 @@
         <v>2580.8300000000004</v>
       </c>
       <c r="G26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.5808300000000002</v>
       </c>
       <c r="H26" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.5808300000000001E-3</v>
       </c>
       <c r="L26">
@@ -1541,15 +1652,15 @@
         <v>4.0509259259259257E-3</v>
       </c>
       <c r="O26">
-        <f>(L26)/($P$20)</f>
+        <f t="shared" si="0"/>
         <v>87.5</v>
       </c>
       <c r="P26">
-        <f>(M26)/($P$20)</f>
+        <f t="shared" si="0"/>
         <v>2.4305555555555556E-2</v>
       </c>
       <c r="Q26">
-        <f>(N26)/($P$20)</f>
+        <f t="shared" si="0"/>
         <v>1.0127314814814814E-3</v>
       </c>
     </row>
@@ -1566,11 +1677,11 @@
         <v>0</v>
       </c>
       <c r="D27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E27" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F27">
@@ -1578,11 +1689,11 @@
         <v>604414.70000000007</v>
       </c>
       <c r="G27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>604.41470000000004</v>
       </c>
       <c r="H27" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.60441470000000008</v>
       </c>
       <c r="I27">
@@ -1610,15 +1721,15 @@
         <v>1.6008101851851853</v>
       </c>
       <c r="O27">
-        <f>(L27)/($P$20)</f>
+        <f t="shared" si="0"/>
         <v>34577.5</v>
       </c>
       <c r="P27">
-        <f>(M27)/($P$20)</f>
+        <f t="shared" si="0"/>
         <v>9.6048611111111111</v>
       </c>
       <c r="Q27">
-        <f>(N27)/($P$20)</f>
+        <f t="shared" si="0"/>
         <v>0.40020254629629631</v>
       </c>
     </row>
@@ -1632,11 +1743,11 @@
         <v>0</v>
       </c>
       <c r="D28" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E28" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F28" s="4">
@@ -1644,11 +1755,11 @@
         <v>606995.53</v>
       </c>
       <c r="G28" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>606.99553000000003</v>
       </c>
       <c r="H28" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.60699553000000006</v>
       </c>
       <c r="L28" s="4">
@@ -1656,11 +1767,11 @@
         <v>138660</v>
       </c>
       <c r="M28" s="5">
-        <f t="shared" ref="M28:N28" si="2">SUM(M24:M27)</f>
+        <f t="shared" ref="M28:N28" si="3">SUM(M24:M27)</f>
         <v>38.516666666666666</v>
       </c>
       <c r="N28" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.6048611111111111</v>
       </c>
       <c r="O28" s="4">
@@ -1668,11 +1779,11 @@
         <v>34665</v>
       </c>
       <c r="P28" s="5">
-        <f t="shared" ref="P28:Q28" si="3">SUM(P24:P27)</f>
+        <f t="shared" ref="P28:Q28" si="4">SUM(P24:P27)</f>
         <v>9.6291666666666664</v>
       </c>
       <c r="Q28" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.40121527777777777</v>
       </c>
     </row>
@@ -1693,11 +1804,11 @@
         <v>0</v>
       </c>
       <c r="D31">
-        <f t="shared" ref="D31:E31" si="4">C31/1000</f>
+        <f t="shared" ref="D31:E31" si="5">C31/1000</f>
         <v>0</v>
       </c>
       <c r="E31" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -1719,11 +1830,11 @@
         <v>0</v>
       </c>
       <c r="D34">
-        <f t="shared" ref="D34:E35" si="5">C34/1000</f>
+        <f t="shared" ref="D34:E35" si="6">C34/1000</f>
         <v>0</v>
       </c>
       <c r="E34" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -1740,11 +1851,11 @@
         <v>0</v>
       </c>
       <c r="D35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E35" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -1765,4 +1876,1583 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9BEF285-D1A0-4C54-AEAA-B385B9C89DCE}">
+  <dimension ref="A2:Q48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="26.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" t="s">
+        <v>40</v>
+      </c>
+      <c r="L3" t="s">
+        <v>39</v>
+      </c>
+      <c r="M3" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P3" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" t="s">
+        <v>27</v>
+      </c>
+      <c r="M4" t="s">
+        <v>0</v>
+      </c>
+      <c r="N4" t="s">
+        <v>22</v>
+      </c>
+      <c r="O4" t="s">
+        <v>23</v>
+      </c>
+      <c r="P4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5">
+        <f>0.00002/5</f>
+        <v>4.0000000000000007E-6</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="H5">
+        <f>IF($B5=$H$2,C5,"")</f>
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <f t="shared" ref="I5:L5" si="0">IF($B5=$H$2,D5,"")</f>
+        <v>4.0000000000000007E-6</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M5" t="str">
+        <f>IF($B5=$M$2,C5,"")</f>
+        <v/>
+      </c>
+      <c r="N5" t="str">
+        <f t="shared" ref="N5:Q5" si="1">IF($B5=$M$2,D5,"")</f>
+        <v/>
+      </c>
+      <c r="O5" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P5" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="Q5" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6">
+        <v>7.9015000000000002E-2</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="H6" t="str">
+        <f t="shared" ref="H6:H14" si="2">IF($B6=$H$2,C6,"")</f>
+        <v/>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" ref="I6:I14" si="3">IF($B6=$H$2,D6,"")</f>
+        <v/>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" ref="J6:J14" si="4">IF($B6=$H$2,E6,"")</f>
+        <v/>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" ref="K6:K14" si="5">IF($B6=$H$2,F6,"")</f>
+        <v/>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" ref="L6:L14" si="6">IF($B6=$H$2,G6,"")</f>
+        <v/>
+      </c>
+      <c r="M6">
+        <f t="shared" ref="M6:M14" si="7">IF($B6=$M$2,C6,"")</f>
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <f t="shared" ref="N6:N14" si="8">IF($B6=$M$2,D6,"")</f>
+        <v>7.9015000000000002E-2</v>
+      </c>
+      <c r="O6">
+        <f t="shared" ref="O6:O14" si="9">IF($B6=$M$2,E6,"")</f>
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <f t="shared" ref="P6:P14" si="10">IF($B6=$M$2,F6,"")</f>
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" ref="Q6:Q14" si="11">IF($B6=$M$2,G6,"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2E-3</v>
+      </c>
+      <c r="G7">
+        <v>1E-3</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="5"/>
+        <v>2E-3</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="6"/>
+        <v>1E-3</v>
+      </c>
+      <c r="M7" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="N7" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="O7" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="P7" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="Q7" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="M8">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="10"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="1">
+        <v>2E-3</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="5"/>
+        <v>2E-3</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M9" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="N9" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="O9" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="P9" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="Q9" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="M10">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="10"/>
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="1">
+        <v>4.403E-2</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="5"/>
+        <v>4.403E-2</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M11" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="N11" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="O11" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="P11" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="Q11" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="1">
+        <v>5.8040000000000001E-2</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="L12" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="M12">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="10"/>
+        <v>5.8040000000000001E-2</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="1">
+        <v>2.452E-2</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="5"/>
+        <v>2.452E-2</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M13" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="N13" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="O13" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="P13" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="Q13" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="1">
+        <v>2.852E-2</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K14" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="L14" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="M14">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="10"/>
+        <v>2.852E-2</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B15" s="1"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B16" s="1"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B17" s="1"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B19" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B25" s="1"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="1">
+        <v>10</v>
+      </c>
+      <c r="P26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C27" t="s">
+        <v>50</v>
+      </c>
+      <c r="L27" t="s">
+        <v>41</v>
+      </c>
+      <c r="O27" t="s">
+        <v>42</v>
+      </c>
+      <c r="P27">
+        <f>$P$26</f>
+        <v>4</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" t="s">
+        <v>23</v>
+      </c>
+      <c r="L28" t="s">
+        <v>27</v>
+      </c>
+      <c r="O28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" t="s">
+        <v>18</v>
+      </c>
+      <c r="F29" t="s">
+        <v>22</v>
+      </c>
+      <c r="G29" t="s">
+        <v>17</v>
+      </c>
+      <c r="H29" t="s">
+        <v>18</v>
+      </c>
+      <c r="I29" t="s">
+        <v>25</v>
+      </c>
+      <c r="J29" t="s">
+        <v>24</v>
+      </c>
+      <c r="K29" t="s">
+        <v>26</v>
+      </c>
+      <c r="L29" t="s">
+        <v>25</v>
+      </c>
+      <c r="M29" t="s">
+        <v>24</v>
+      </c>
+      <c r="N29" t="s">
+        <v>26</v>
+      </c>
+      <c r="O29" t="s">
+        <v>25</v>
+      </c>
+      <c r="P29" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <f>$B30*SUMIF($A$5:$A$18,$A30,$C$5:$C$18)</f>
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <f>C30/1000</f>
+        <v>0</v>
+      </c>
+      <c r="E30" s="2">
+        <f>D30/1000</f>
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <f>$B30*SUMIF($A$5:$A$18,$A30,$D$5:$D$18)</f>
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <f>F30/1000</f>
+        <v>0</v>
+      </c>
+      <c r="H30" s="2">
+        <f>G30/1000</f>
+        <v>0</v>
+      </c>
+      <c r="O30">
+        <f t="shared" ref="O30:Q35" si="12">(L30)/($P$26)</f>
+        <v>0</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31">
+        <v>13831</v>
+      </c>
+      <c r="C31">
+        <f>$B31*SUMIF($A$5:$A$18,$A31,$C$5:$C$18)</f>
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <f t="shared" ref="D31:E36" si="13">C31/1000</f>
+        <v>0</v>
+      </c>
+      <c r="E31" s="2">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <f>$B31*SUMIF($A$5:$A$18,$A31,$D$5:$D$18)</f>
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <f t="shared" ref="G31:H36" si="14">F31/1000</f>
+        <v>0</v>
+      </c>
+      <c r="H31" s="2">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="Q31">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32">
+        <v>1000</v>
+      </c>
+      <c r="C32">
+        <f>$B32*SUMIF($A$5:$A$18,$A32,$C$5:$C$18)</f>
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="E32" s="2">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <f>$B32*SUMIF($A$5:$A$18,$A32,$D$5:$D$18)</f>
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="H32" s="2">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <f>$B32*SUMIF($A$5:$A$18,$A32,$F$5:$F$18)</f>
+        <v>53.040000000000006</v>
+      </c>
+      <c r="M32" s="6">
+        <f>L32/3600</f>
+        <v>1.4733333333333334E-2</v>
+      </c>
+      <c r="N32" s="6">
+        <f>M32/24</f>
+        <v>6.1388888888888897E-4</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="12"/>
+        <v>13.260000000000002</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="12"/>
+        <v>3.6833333333333336E-3</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" si="12"/>
+        <v>1.5347222222222224E-4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33">
+        <f>B35*$B$26</f>
+        <v>138310000</v>
+      </c>
+      <c r="C33">
+        <f>$B33*SUMIF($A$5:$A$18,$A33,$C$5:$C$18)</f>
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <f t="shared" ref="D33" si="15">C33/1000</f>
+        <v>0</v>
+      </c>
+      <c r="E33" s="2">
+        <f t="shared" ref="E33" si="16">D33/1000</f>
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <f>$B33*SUMIF($A$5:$A$18,$A33,$D$5:$D$18)</f>
+        <v>10929117.890000001</v>
+      </c>
+      <c r="G33">
+        <f t="shared" ref="G33" si="17">F33/1000</f>
+        <v>10929.117890000001</v>
+      </c>
+      <c r="H33" s="2">
+        <f t="shared" ref="H33" si="18">G33/1000</f>
+        <v>10.929117890000001</v>
+      </c>
+      <c r="L33">
+        <f>$B33*SUMIF($A$5:$A$18,$A33,$F$5:$F$18)</f>
+        <v>3734370.0000000005</v>
+      </c>
+      <c r="M33" s="6">
+        <f>L33/3600</f>
+        <v>1037.325</v>
+      </c>
+      <c r="N33" s="6">
+        <f>M33/24</f>
+        <v>43.221875000000004</v>
+      </c>
+      <c r="O33">
+        <f t="shared" ref="O33" si="19">(L33)/($P$26)</f>
+        <v>933592.50000000012</v>
+      </c>
+      <c r="P33">
+        <f t="shared" ref="P33" si="20">(M33)/($P$26)</f>
+        <v>259.33125000000001</v>
+      </c>
+      <c r="Q33">
+        <f t="shared" ref="Q33" si="21">(N33)/($P$26)</f>
+        <v>10.805468750000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="E34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="M34" s="6"/>
+      <c r="N34" s="6"/>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35">
+        <f>B31*B32</f>
+        <v>13831000</v>
+      </c>
+      <c r="C35">
+        <f>$B35*SUMIF($A$5:$A$18,$A35,$C$5:$C$18)</f>
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="E35" s="2">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <f>$B35*SUMIF($A$5:$A$18,$A35,$D$5:$D$18)</f>
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="H35" s="2">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <f>$B35*SUMIF($A$5:$A$18,$A35,$E$5:$E$18)</f>
+        <v>0</v>
+      </c>
+      <c r="J35" s="6">
+        <f>I35/3600</f>
+        <v>0</v>
+      </c>
+      <c r="K35" s="6">
+        <f>J35/24</f>
+        <v>0</v>
+      </c>
+      <c r="L35">
+        <f>$B35*SUMIF($A$5:$A$18,$A35,$F$5:$F$18)</f>
+        <v>414930</v>
+      </c>
+      <c r="M35" s="6">
+        <f>L35/3600</f>
+        <v>115.25833333333334</v>
+      </c>
+      <c r="N35" s="6">
+        <f>M35/24</f>
+        <v>4.8024305555555555</v>
+      </c>
+      <c r="O35">
+        <f t="shared" si="12"/>
+        <v>103732.5</v>
+      </c>
+      <c r="P35">
+        <f t="shared" si="12"/>
+        <v>28.814583333333335</v>
+      </c>
+      <c r="Q35">
+        <f t="shared" si="12"/>
+        <v>1.2006076388888889</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4">
+        <f>SUM(C30:C35)</f>
+        <v>0</v>
+      </c>
+      <c r="D36" s="4">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="E36" s="5">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="F36" s="4">
+        <f>SUM(F30:F35)</f>
+        <v>10929117.890000001</v>
+      </c>
+      <c r="G36" s="4">
+        <f t="shared" si="14"/>
+        <v>10929.117890000001</v>
+      </c>
+      <c r="H36" s="5">
+        <f t="shared" si="14"/>
+        <v>10.929117890000001</v>
+      </c>
+      <c r="L36" s="4">
+        <f>SUM(L30:L35)</f>
+        <v>4149353.0400000005</v>
+      </c>
+      <c r="M36" s="5">
+        <f t="shared" ref="M36:N36" si="22">SUM(M30:M35)</f>
+        <v>1152.5980666666669</v>
+      </c>
+      <c r="N36" s="5">
+        <f t="shared" si="22"/>
+        <v>48.024919444444443</v>
+      </c>
+      <c r="O36" s="4">
+        <f>SUM(O30:O35)</f>
+        <v>1037338.2600000001</v>
+      </c>
+      <c r="P36" s="5">
+        <f t="shared" ref="P36:Q36" si="23">SUM(P30:P35)</f>
+        <v>288.14951666666673</v>
+      </c>
+      <c r="Q36" s="5">
+        <f t="shared" si="23"/>
+        <v>12.006229861111111</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C39" t="s">
+        <v>52</v>
+      </c>
+      <c r="L39" t="s">
+        <v>41</v>
+      </c>
+      <c r="O39" t="s">
+        <v>42</v>
+      </c>
+      <c r="P39">
+        <f>P27</f>
+        <v>4</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C40" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" t="s">
+        <v>23</v>
+      </c>
+      <c r="L40" t="s">
+        <v>27</v>
+      </c>
+      <c r="O40" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>16</v>
+      </c>
+      <c r="C41" t="s">
+        <v>0</v>
+      </c>
+      <c r="D41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E41" t="s">
+        <v>18</v>
+      </c>
+      <c r="F41" t="s">
+        <v>22</v>
+      </c>
+      <c r="G41" t="s">
+        <v>17</v>
+      </c>
+      <c r="H41" t="s">
+        <v>18</v>
+      </c>
+      <c r="I41" t="s">
+        <v>25</v>
+      </c>
+      <c r="J41" t="s">
+        <v>24</v>
+      </c>
+      <c r="K41" t="s">
+        <v>26</v>
+      </c>
+      <c r="L41" t="s">
+        <v>25</v>
+      </c>
+      <c r="M41" t="s">
+        <v>24</v>
+      </c>
+      <c r="N41" t="s">
+        <v>26</v>
+      </c>
+      <c r="O41" t="s">
+        <v>25</v>
+      </c>
+      <c r="P41" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>11</v>
+      </c>
+      <c r="B42">
+        <f>B30</f>
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <f>$B42*SUMIF($A$5:$A$18,$A42,$H$5:$H$18)</f>
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <f>C42/1000</f>
+        <v>0</v>
+      </c>
+      <c r="E42" s="2">
+        <f>D42/1000</f>
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <f>$B42*SUMIF($A$5:$A$18,$A42,$I$5:$I$18)</f>
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <f>F42/1000</f>
+        <v>0</v>
+      </c>
+      <c r="H42" s="2">
+        <f>G42/1000</f>
+        <v>0</v>
+      </c>
+      <c r="L42">
+        <f t="shared" ref="L42:L43" si="24">$B42*SUMIF($A$5:$A$18,$A42,$K$5:$K$18)</f>
+        <v>0</v>
+      </c>
+      <c r="M42" s="6">
+        <f t="shared" ref="M42:M43" si="25">L42/3600</f>
+        <v>0</v>
+      </c>
+      <c r="N42" s="6">
+        <f t="shared" ref="N42:N43" si="26">M42/24</f>
+        <v>0</v>
+      </c>
+      <c r="O42">
+        <f t="shared" ref="O42:O47" si="27">(L42)/($P$26)</f>
+        <v>0</v>
+      </c>
+      <c r="P42">
+        <f t="shared" ref="P42:P47" si="28">(M42)/($P$26)</f>
+        <v>0</v>
+      </c>
+      <c r="Q42">
+        <f t="shared" ref="Q42:Q47" si="29">(N42)/($P$26)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>12</v>
+      </c>
+      <c r="B43">
+        <f t="shared" ref="B43:B47" si="30">B31</f>
+        <v>13831</v>
+      </c>
+      <c r="C43">
+        <f t="shared" ref="C43:C45" si="31">$B43*SUMIF($A$5:$A$18,$A43,$H$5:$H$18)</f>
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <f t="shared" ref="D43:D48" si="32">C43/1000</f>
+        <v>0</v>
+      </c>
+      <c r="E43" s="2">
+        <f t="shared" ref="E43:E48" si="33">D43/1000</f>
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <f t="shared" ref="F43:F47" si="34">$B43*SUMIF($A$5:$A$18,$A43,$I$5:$I$18)</f>
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <f t="shared" ref="G43:G48" si="35">F43/1000</f>
+        <v>0</v>
+      </c>
+      <c r="H43" s="2">
+        <f t="shared" ref="H43:H48" si="36">G43/1000</f>
+        <v>0</v>
+      </c>
+      <c r="L43">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="M43" s="6">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="N43" s="6">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="O43">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="P43">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="Q43">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>13</v>
+      </c>
+      <c r="B44">
+        <f t="shared" si="30"/>
+        <v>1000</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="E44" s="2">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="H44" s="2">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="L44">
+        <f>$B44*SUMIF($A$5:$A$18,$A44,$K$5:$K$18)</f>
+        <v>24.52</v>
+      </c>
+      <c r="M44" s="6">
+        <f>L44/3600</f>
+        <v>6.8111111111111107E-3</v>
+      </c>
+      <c r="N44" s="6">
+        <f>M44/24</f>
+        <v>2.8379629629629626E-4</v>
+      </c>
+      <c r="O44">
+        <f t="shared" si="27"/>
+        <v>6.13</v>
+      </c>
+      <c r="P44">
+        <f t="shared" si="28"/>
+        <v>1.7027777777777777E-3</v>
+      </c>
+      <c r="Q44">
+        <f t="shared" si="29"/>
+        <v>7.0949074074074065E-5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>45</v>
+      </c>
+      <c r="B45">
+        <f t="shared" si="30"/>
+        <v>138310000</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="E45" s="2">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="34"/>
+        <v>553.24000000000012</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="35"/>
+        <v>0.55324000000000018</v>
+      </c>
+      <c r="H45" s="2">
+        <f t="shared" si="36"/>
+        <v>5.532400000000002E-4</v>
+      </c>
+      <c r="L45">
+        <f t="shared" ref="L45:L47" si="37">$B45*SUMIF($A$5:$A$18,$A45,$K$5:$K$18)</f>
+        <v>276620</v>
+      </c>
+      <c r="M45" s="6">
+        <f t="shared" ref="M45:M47" si="38">L45/3600</f>
+        <v>76.838888888888889</v>
+      </c>
+      <c r="N45" s="6">
+        <f t="shared" ref="N45:N47" si="39">M45/24</f>
+        <v>3.2016203703703705</v>
+      </c>
+      <c r="O45">
+        <f t="shared" si="27"/>
+        <v>69155</v>
+      </c>
+      <c r="P45">
+        <f t="shared" si="28"/>
+        <v>19.209722222222222</v>
+      </c>
+      <c r="Q45">
+        <f t="shared" si="29"/>
+        <v>0.80040509259259263</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>46</v>
+      </c>
+      <c r="B46">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
+      <c r="E46" s="2"/>
+      <c r="F46">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="H46" s="2"/>
+      <c r="L46">
+        <f t="shared" si="37"/>
+        <v>4.403E-2</v>
+      </c>
+      <c r="M46" s="6">
+        <f t="shared" si="38"/>
+        <v>1.2230555555555555E-5</v>
+      </c>
+      <c r="N46" s="6">
+        <f t="shared" si="39"/>
+        <v>5.0960648148148144E-7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>14</v>
+      </c>
+      <c r="B47">
+        <f t="shared" si="30"/>
+        <v>13831000</v>
+      </c>
+      <c r="C47">
+        <f>$B47*SUMIF($A$5:$A$18,$A47,$C$5:$C$18)</f>
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <f t="shared" ref="D47:D48" si="40">C47/1000</f>
+        <v>0</v>
+      </c>
+      <c r="E47" s="2">
+        <f t="shared" ref="E47:E48" si="41">D47/1000</f>
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <f t="shared" ref="G47:G48" si="42">F47/1000</f>
+        <v>0</v>
+      </c>
+      <c r="H47" s="2">
+        <f t="shared" ref="H47:H48" si="43">G47/1000</f>
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <f>$B47*SUMIF($A$5:$A$18,$A47,$E$5:$E$18)</f>
+        <v>0</v>
+      </c>
+      <c r="J47" s="6">
+        <f>I47/3600</f>
+        <v>0</v>
+      </c>
+      <c r="K47" s="6">
+        <f>J47/24</f>
+        <v>0</v>
+      </c>
+      <c r="L47">
+        <f t="shared" si="37"/>
+        <v>27662</v>
+      </c>
+      <c r="M47" s="6">
+        <f t="shared" si="38"/>
+        <v>7.6838888888888892</v>
+      </c>
+      <c r="N47" s="6">
+        <f t="shared" si="39"/>
+        <v>0.32016203703703705</v>
+      </c>
+      <c r="O47">
+        <f t="shared" ref="O47:O48" si="44">(L47)/($P$26)</f>
+        <v>6915.5</v>
+      </c>
+      <c r="P47">
+        <f t="shared" ref="P47:P48" si="45">(M47)/($P$26)</f>
+        <v>1.9209722222222223</v>
+      </c>
+      <c r="Q47">
+        <f t="shared" ref="Q47:Q48" si="46">(N47)/($P$26)</f>
+        <v>8.0040509259259263E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4">
+        <f>SUM(C42:C47)</f>
+        <v>0</v>
+      </c>
+      <c r="D48" s="4">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="E48" s="5">
+        <f t="shared" si="41"/>
+        <v>0</v>
+      </c>
+      <c r="F48" s="4">
+        <f>SUM(F42:F47)</f>
+        <v>553.24000000000012</v>
+      </c>
+      <c r="G48" s="4">
+        <f t="shared" si="42"/>
+        <v>0.55324000000000018</v>
+      </c>
+      <c r="H48" s="5">
+        <f t="shared" si="43"/>
+        <v>5.532400000000002E-4</v>
+      </c>
+      <c r="L48" s="4">
+        <f>SUM(L42:L47)</f>
+        <v>304306.56403000001</v>
+      </c>
+      <c r="M48" s="5">
+        <f t="shared" ref="M48:N48" si="47">SUM(M42:M47)</f>
+        <v>84.529601119444436</v>
+      </c>
+      <c r="N48" s="5">
+        <f t="shared" si="47"/>
+        <v>3.5220667133101857</v>
+      </c>
+      <c r="O48" s="4">
+        <f>SUM(O42:O47)</f>
+        <v>76076.63</v>
+      </c>
+      <c r="P48" s="5">
+        <f t="shared" ref="P48:Q48" si="48">SUM(P42:P47)</f>
+        <v>21.13239722222222</v>
+      </c>
+      <c r="Q48" s="5">
+        <f t="shared" si="48"/>
+        <v>0.88051655092592607</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="F40:H40"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="F28:H28"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updates MC LCI and LCA
</commit_message>
<xml_diff>
--- a/Calculation time and size.xlsx
+++ b/Calculation time and size.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="10212" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -157,12 +157,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="C55" authorId="0" shapeId="0" xr:uid="{3E0D0EFB-8CCB-4BB3-AAF4-5FE7B6F5704F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+First iteration --&gt; creation of everything so longer</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="86">
   <si>
     <t>Storage size in HDF5 [MB]</t>
   </si>
@@ -321,13 +345,112 @@
   </si>
   <si>
     <t>For aggregated</t>
+  </si>
+  <si>
+    <t>8h</t>
+  </si>
+  <si>
+    <t>27 iterations</t>
+  </si>
+  <si>
+    <t>4 cpus</t>
+  </si>
+  <si>
+    <t>h/iteration</t>
+  </si>
+  <si>
+    <t>iteration</t>
+  </si>
+  <si>
+    <t>days</t>
+  </si>
+  <si>
+    <t>observed data</t>
+  </si>
+  <si>
+    <t>GB/iteration/cpu</t>
+  </si>
+  <si>
+    <t>My computer</t>
+  </si>
+  <si>
+    <t>Gael computer</t>
+  </si>
+  <si>
+    <t>h of run</t>
+  </si>
+  <si>
+    <t>iteration for one cpu</t>
+  </si>
+  <si>
+    <t>total iteration</t>
+  </si>
+  <si>
+    <t>Gathering function</t>
+  </si>
+  <si>
+    <t>Cleaning</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>[sec]/iteration/all DB/worker</t>
+  </si>
+  <si>
+    <t>Gathering</t>
+  </si>
+  <si>
+    <t>calculated</t>
+  </si>
+  <si>
+    <t>[sec]/all DB</t>
+  </si>
+  <si>
+    <t>[h]/all DB</t>
+  </si>
+  <si>
+    <t>[min]/all DB</t>
+  </si>
+  <si>
+    <t>iterations</t>
+  </si>
+  <si>
+    <t>Deterministic LCI</t>
+  </si>
+  <si>
+    <t>For the all DB</t>
+  </si>
+  <si>
+    <t>[sec/DB]</t>
+  </si>
+  <si>
+    <t>Aggregated LCA</t>
+  </si>
+  <si>
+    <t>[sec/DB/iteration]</t>
+  </si>
+  <si>
+    <t>[min/DB/iteration]</t>
+  </si>
+  <si>
+    <t>Processeur</t>
+  </si>
+  <si>
+    <t>[h/DB/iteration]</t>
+  </si>
+  <si>
+    <t>iterations total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -370,6 +493,35 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -391,7 +543,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -404,6 +556,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1240,631 +1404,964 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5E8E4FE-D9C4-4A09-8B44-2D595489B0E8}">
-  <dimension ref="A3:Q37"/>
+  <dimension ref="A2:Q53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD28"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" customWidth="1"/>
-    <col min="2" max="2" width="18.109375" customWidth="1"/>
-    <col min="3" max="3" width="23.44140625" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" style="8" customWidth="1"/>
+    <col min="3" max="3" width="23.44140625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="8"/>
+    <col min="5" max="5" width="10.109375" style="8" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="8"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C3" t="s">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="I2" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="8" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
+      <c r="I3" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="C4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="8" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="I4" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="O4" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="P4" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q4" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="F5" s="9"/>
+      <c r="I5" s="8">
+        <v>8</v>
+      </c>
+      <c r="J5" s="8">
+        <v>27</v>
+      </c>
+      <c r="K5" s="8">
+        <v>4</v>
+      </c>
+      <c r="L5" s="8">
+        <v>64</v>
+      </c>
+      <c r="N5" s="8">
+        <v>8</v>
+      </c>
+      <c r="O5" s="8">
+        <v>27</v>
+      </c>
+      <c r="P5" s="8">
+        <v>4</v>
+      </c>
+      <c r="Q5" s="8">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="F6" s="9"/>
+      <c r="I6" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="N6" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="O6" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="P6" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="F7" s="9"/>
+      <c r="I7" s="8">
+        <f>I5/J5</f>
+        <v>0.29629629629629628</v>
+      </c>
+      <c r="J7" s="8">
+        <v>63</v>
+      </c>
+      <c r="K7" s="8">
+        <f>I7*J7/24</f>
+        <v>0.77777777777777768</v>
+      </c>
+      <c r="N7" s="8">
+        <f>N5/O5</f>
+        <v>0.29629629629629628</v>
+      </c>
+      <c r="O7" s="8">
+        <v>1000</v>
+      </c>
+      <c r="P7" s="8">
+        <f>N7*O7/24</f>
+        <v>12.345679012345679</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="8">
         <f>1.7375</f>
         <v>1.7375</v>
       </c>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="F8" s="9"/>
+      <c r="I8" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="N8" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="P8" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="F9" s="9"/>
+      <c r="I9" s="8">
+        <f>L5/J5/K5</f>
+        <v>0.59259259259259256</v>
+      </c>
+      <c r="J9" s="8">
+        <f>J7</f>
+        <v>63</v>
+      </c>
+      <c r="K9" s="8">
+        <f>I9*J9</f>
+        <v>37.333333333333329</v>
+      </c>
+      <c r="N9" s="8">
+        <f>Q5/O5/P5</f>
+        <v>0.59259259259259256</v>
+      </c>
+      <c r="O9" s="8">
+        <f>O7</f>
+        <v>1000</v>
+      </c>
+      <c r="P9" s="8">
+        <f>N9*O9</f>
+        <v>592.59259259259261</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="F10" s="9"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="8">
         <f>43700/1000000</f>
         <v>4.3700000000000003E-2</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="9">
         <v>0.01</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="8">
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="8">
         <f>0.84333</f>
         <v>0.84333000000000002</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="8">
         <v>0.35</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="8">
         <v>0.27</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B13" s="1" t="s">
+      <c r="I12" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B13" s="9" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B14" s="1"/>
-      <c r="C14" t="s">
+      <c r="I13" s="8">
+        <f>I7</f>
+        <v>0.29629629629629628</v>
+      </c>
+      <c r="J13" s="8">
+        <v>8</v>
+      </c>
+      <c r="K13" s="8">
+        <f>J13/I13</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B14" s="9"/>
+      <c r="C14" s="8" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="K14" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="9" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="K15" s="8">
+        <f>K13*K5</f>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="9" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="A17" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="A18" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="9" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B19" s="1"/>
+      <c r="B19" s="9"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B20" s="1"/>
-      <c r="P20">
+      <c r="B20" s="9"/>
+      <c r="P20" s="8">
         <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="L21" t="s">
+      <c r="L21" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="O21" t="s">
+      <c r="O21" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="P21">
+      <c r="P21" s="8">
         <f>$P$20</f>
         <v>4</v>
       </c>
-      <c r="Q21" t="s">
+      <c r="Q21" s="8" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7" t="s">
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" t="s">
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="L22" t="s">
+      <c r="L22" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="O22" t="s">
+      <c r="O22" s="8" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
+      <c r="B23" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C23" t="s">
-        <v>0</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="C23" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H23" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="I23" t="s">
+      <c r="I23" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="J23" t="s">
+      <c r="J23" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="K23" t="s">
+      <c r="K23" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="L23" t="s">
+      <c r="L23" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="M23" t="s">
+      <c r="M23" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="N23" t="s">
+      <c r="N23" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="O23" t="s">
+      <c r="O23" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="P23" t="s">
+      <c r="P23" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="Q23" t="s">
+      <c r="Q23" s="8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="A24" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="8">
         <v>1</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="8">
         <f>$B24*SUMIF($A$5:$A$12,$A24,$C$5:$C$12)</f>
         <v>0</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="8">
         <f>C24/1000</f>
         <v>0</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24" s="12">
         <f>D24/1000</f>
         <v>0</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="8">
         <f>$B24*SUMIF($A$5:$A$12,$A24,$D$5:$D$12)</f>
         <v>0</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="8">
         <f>F24/1000</f>
         <v>0</v>
       </c>
-      <c r="H24" s="2">
+      <c r="H24" s="12">
         <f>G24/1000</f>
         <v>0</v>
       </c>
-      <c r="O24">
+      <c r="O24" s="8">
         <f t="shared" ref="O24:Q27" si="0">(L24)/($P$20)</f>
         <v>0</v>
       </c>
-      <c r="P24">
+      <c r="P24" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q24">
+      <c r="Q24" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="A25" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="8">
         <v>13831</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="8">
         <f>$B25*SUMIF($A$5:$A$12,$A25,$C$5:$C$12)</f>
         <v>0</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="8">
         <f t="shared" ref="D25:E28" si="1">C25/1000</f>
         <v>0</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="8">
         <f>$B25*SUMIF($A$5:$A$12,$A25,$D$5:$D$12)</f>
         <v>0</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="8">
         <f t="shared" ref="G25:H28" si="2">F25/1000</f>
         <v>0</v>
       </c>
-      <c r="H25" s="2">
+      <c r="H25" s="12">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O25">
+      <c r="O25" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P25">
+      <c r="P25" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q25">
+      <c r="Q25" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="A26" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="8">
         <v>1000</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="8">
         <f>$B26*SUMIF($A$5:$A$12,$A26,$C$5:$C$12)</f>
         <v>0</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="8">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E26" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="8">
         <f>$B26*SUMIF($A$5:$A$12,$A26,$D$5:$D$12)</f>
         <v>2580.8300000000004</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="8">
         <f t="shared" si="2"/>
         <v>2.5808300000000002</v>
       </c>
-      <c r="H26" s="2">
+      <c r="H26" s="12">
         <f t="shared" si="2"/>
         <v>2.5808300000000001E-3</v>
       </c>
-      <c r="L26">
+      <c r="L26" s="8">
         <f>$B26*SUMIF($A$5:$A$12,$A26,$F$5:$F$12)</f>
         <v>350</v>
       </c>
-      <c r="M26" s="6">
+      <c r="M26" s="13">
         <f>L26/3600</f>
         <v>9.7222222222222224E-2</v>
       </c>
-      <c r="N26" s="6">
+      <c r="N26" s="13">
         <f>M26/24</f>
         <v>4.0509259259259257E-3</v>
       </c>
-      <c r="O26">
+      <c r="O26" s="8">
         <f t="shared" si="0"/>
         <v>87.5</v>
       </c>
-      <c r="P26">
+      <c r="P26" s="8">
         <f t="shared" si="0"/>
         <v>2.4305555555555556E-2</v>
       </c>
-      <c r="Q26">
+      <c r="Q26" s="8">
         <f t="shared" si="0"/>
         <v>1.0127314814814814E-3</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="A27" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="8">
         <f>B25*B26</f>
         <v>13831000</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="8">
         <f>$B27*SUMIF($A$5:$A$12,$A27,$C$5:$C$12)</f>
         <v>0</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="8">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E27" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="8">
         <f>$B27*SUMIF($A$5:$A$12,$A27,$D$5:$D$12)</f>
         <v>604414.70000000007</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="8">
         <f t="shared" si="2"/>
         <v>604.41470000000004</v>
       </c>
-      <c r="H27" s="2">
+      <c r="H27" s="12">
         <f t="shared" si="2"/>
         <v>0.60441470000000008</v>
       </c>
-      <c r="I27">
+      <c r="I27" s="8">
         <f>$B27*SUMIF($A$5:$A$12,$A27,$E$5:$E$12)</f>
         <v>0</v>
       </c>
-      <c r="J27" s="6">
+      <c r="J27" s="13">
         <f>I27/3600</f>
         <v>0</v>
       </c>
-      <c r="K27" s="6">
+      <c r="K27" s="13">
         <f>J27/24</f>
         <v>0</v>
       </c>
-      <c r="L27">
+      <c r="L27" s="8">
         <f>$B27*SUMIF($A$5:$A$12,$A27,$F$5:$F$12)</f>
         <v>138310</v>
       </c>
-      <c r="M27" s="6">
+      <c r="M27" s="13">
         <f>L27/3600</f>
         <v>38.419444444444444</v>
       </c>
-      <c r="N27" s="6">
+      <c r="N27" s="13">
         <f>M27/24</f>
         <v>1.6008101851851853</v>
       </c>
-      <c r="O27">
+      <c r="O27" s="8">
         <f t="shared" si="0"/>
         <v>34577.5</v>
       </c>
-      <c r="P27">
+      <c r="P27" s="8">
         <f t="shared" si="0"/>
         <v>9.6048611111111111</v>
       </c>
-      <c r="Q27">
+      <c r="Q27" s="8">
         <f t="shared" si="0"/>
         <v>0.40020254629629631</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4">
+      <c r="B28" s="14"/>
+      <c r="C28" s="14">
         <f>SUM(C24:C27)</f>
         <v>0</v>
       </c>
-      <c r="D28" s="4">
+      <c r="D28" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E28" s="5">
+      <c r="E28" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F28" s="4">
+      <c r="F28" s="14">
         <f>SUM(F24:F27)</f>
         <v>606995.53</v>
       </c>
-      <c r="G28" s="4">
+      <c r="G28" s="14">
         <f t="shared" si="2"/>
         <v>606.99553000000003</v>
       </c>
-      <c r="H28" s="5">
+      <c r="H28" s="15">
         <f t="shared" si="2"/>
         <v>0.60699553000000006</v>
       </c>
-      <c r="L28" s="4">
+      <c r="L28" s="14">
         <f>SUM(L24:L27)</f>
         <v>138660</v>
       </c>
-      <c r="M28" s="5">
+      <c r="M28" s="15">
         <f t="shared" ref="M28:N28" si="3">SUM(M24:M27)</f>
         <v>38.516666666666666</v>
       </c>
-      <c r="N28" s="5">
+      <c r="N28" s="15">
         <f t="shared" si="3"/>
         <v>1.6048611111111111</v>
       </c>
-      <c r="O28" s="4">
+      <c r="O28" s="14">
         <f>SUM(O24:O27)</f>
         <v>34665</v>
       </c>
-      <c r="P28" s="5">
+      <c r="P28" s="15">
         <f t="shared" ref="P28:Q28" si="4">SUM(P24:P27)</f>
         <v>9.6291666666666664</v>
       </c>
-      <c r="Q28" s="5">
+      <c r="Q28" s="15">
         <f t="shared" si="4"/>
         <v>0.40121527777777777</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="H29" s="2"/>
+      <c r="H29" s="12"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="A30" s="8" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+      <c r="A31" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="8">
         <f>B27*C15</f>
         <v>0</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="8">
         <f t="shared" ref="D31:E31" si="5">C31/1000</f>
         <v>0</v>
       </c>
-      <c r="E31" s="2">
+      <c r="E31" s="12">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+      <c r="A33" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+      <c r="A34" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="8">
         <f>B26</f>
         <v>1000</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="8">
         <f>B34*(C16+C18)</f>
         <v>0</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="8">
         <f t="shared" ref="D34:E35" si="6">C34/1000</f>
         <v>0</v>
       </c>
-      <c r="E34" s="2">
+      <c r="E34" s="12">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+      <c r="A35" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="8">
         <f>B27</f>
         <v>13831000</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="8">
         <f>B35*C17</f>
         <v>0</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="8">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="E35" s="2">
+      <c r="E35" s="12">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+      <c r="A37" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="8" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B41" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B43" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B44" s="8">
+        <f>0.86/2</f>
+        <v>0.43</v>
+      </c>
+      <c r="C44" s="8">
+        <f>110/2</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B45" s="8">
+        <f>78/2</f>
+        <v>39</v>
+      </c>
+      <c r="C45" s="8">
+        <f>137/2</f>
+        <v>68.5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B47" s="8">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B48" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B49" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B50" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="F50" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B51" s="8">
+        <f>B44*$B$47</f>
+        <v>430</v>
+      </c>
+      <c r="C51" s="8">
+        <f>C44*$B$47</f>
+        <v>55000</v>
+      </c>
+      <c r="D51" s="13">
+        <f t="shared" ref="D51:G52" si="7">B51/60</f>
+        <v>7.166666666666667</v>
+      </c>
+      <c r="E51" s="13">
+        <f t="shared" si="7"/>
+        <v>916.66666666666663</v>
+      </c>
+      <c r="F51" s="13">
+        <f t="shared" si="7"/>
+        <v>0.11944444444444445</v>
+      </c>
+      <c r="G51" s="13">
+        <f t="shared" si="7"/>
+        <v>15.277777777777777</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B52" s="8">
+        <f>B45*$B$47</f>
+        <v>39000</v>
+      </c>
+      <c r="C52" s="8">
+        <f>C45*$B$47</f>
+        <v>68500</v>
+      </c>
+      <c r="D52" s="13">
+        <f t="shared" si="7"/>
+        <v>650</v>
+      </c>
+      <c r="E52" s="13">
+        <f t="shared" si="7"/>
+        <v>1141.6666666666667</v>
+      </c>
+      <c r="F52" s="13">
+        <f t="shared" si="7"/>
+        <v>10.833333333333334</v>
+      </c>
+      <c r="G52" s="13">
+        <f t="shared" si="7"/>
+        <v>19.027777777777779</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B53" s="13">
+        <f t="shared" ref="B53:G53" si="8">SUM(B51:B52)</f>
+        <v>39430</v>
+      </c>
+      <c r="C53" s="13">
+        <f t="shared" si="8"/>
+        <v>123500</v>
+      </c>
+      <c r="D53" s="13">
+        <f t="shared" si="8"/>
+        <v>657.16666666666663</v>
+      </c>
+      <c r="E53" s="13">
+        <f t="shared" si="8"/>
+        <v>2058.3333333333335</v>
+      </c>
+      <c r="F53" s="13">
+        <f t="shared" si="8"/>
+        <v>10.952777777777778</v>
+      </c>
+      <c r="G53" s="13">
+        <f t="shared" si="8"/>
+        <v>34.305555555555557</v>
       </c>
     </row>
   </sheetData>
@@ -1880,16 +2377,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9BEF285-D1A0-4C54-AEAA-B385B9C89DCE}">
-  <dimension ref="A2:Q48"/>
+  <dimension ref="A2:Q58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="26.77734375" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
@@ -3112,15 +3611,15 @@
         <v>0</v>
       </c>
       <c r="O42">
-        <f t="shared" ref="O42:O47" si="27">(L42)/($P$26)</f>
+        <f t="shared" ref="O42:O45" si="27">(L42)/($P$26)</f>
         <v>0</v>
       </c>
       <c r="P42">
-        <f t="shared" ref="P42:P47" si="28">(M42)/($P$26)</f>
+        <f t="shared" ref="P42:P45" si="28">(M42)/($P$26)</f>
         <v>0</v>
       </c>
       <c r="Q42">
-        <f t="shared" ref="Q42:Q47" si="29">(N42)/($P$26)</f>
+        <f t="shared" ref="Q42:Q45" si="29">(N42)/($P$26)</f>
         <v>0</v>
       </c>
     </row>
@@ -3137,11 +3636,11 @@
         <v>0</v>
       </c>
       <c r="D43">
-        <f t="shared" ref="D43:D48" si="32">C43/1000</f>
+        <f t="shared" ref="D43:D45" si="32">C43/1000</f>
         <v>0</v>
       </c>
       <c r="E43" s="2">
-        <f t="shared" ref="E43:E48" si="33">D43/1000</f>
+        <f t="shared" ref="E43:E45" si="33">D43/1000</f>
         <v>0</v>
       </c>
       <c r="F43">
@@ -3149,11 +3648,11 @@
         <v>0</v>
       </c>
       <c r="G43">
-        <f t="shared" ref="G43:G48" si="35">F43/1000</f>
+        <f t="shared" ref="G43:G45" si="35">F43/1000</f>
         <v>0</v>
       </c>
       <c r="H43" s="2">
-        <f t="shared" ref="H43:H48" si="36">G43/1000</f>
+        <f t="shared" ref="H43:H45" si="36">G43/1000</f>
         <v>0</v>
       </c>
       <c r="L43">
@@ -3379,15 +3878,15 @@
         <v>0.32016203703703705</v>
       </c>
       <c r="O47">
-        <f t="shared" ref="O47:O48" si="44">(L47)/($P$26)</f>
+        <f t="shared" ref="O47" si="44">(L47)/($P$26)</f>
         <v>6915.5</v>
       </c>
       <c r="P47">
-        <f t="shared" ref="P47:P48" si="45">(M47)/($P$26)</f>
+        <f t="shared" ref="P47" si="45">(M47)/($P$26)</f>
         <v>1.9209722222222223</v>
       </c>
       <c r="Q47">
-        <f t="shared" ref="Q47:Q48" si="46">(N47)/($P$26)</f>
+        <f t="shared" ref="Q47" si="46">(N47)/($P$26)</f>
         <v>8.0040509259259263E-2</v>
       </c>
     </row>
@@ -3443,6 +3942,78 @@
       <c r="Q48" s="5">
         <f t="shared" si="48"/>
         <v>0.88051655092592607</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>77</v>
+      </c>
+      <c r="B53" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>78</v>
+      </c>
+      <c r="B54">
+        <v>5576</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>80</v>
+      </c>
+      <c r="C55">
+        <v>1423</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>85</v>
+      </c>
+      <c r="B56" t="s">
+        <v>83</v>
+      </c>
+      <c r="C56" t="s">
+        <v>81</v>
+      </c>
+      <c r="D56" t="s">
+        <v>82</v>
+      </c>
+      <c r="E56" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>1</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="C57">
+        <v>927</v>
+      </c>
+      <c r="D57">
+        <f>C57/60</f>
+        <v>15.45</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>1000</v>
+      </c>
+      <c r="B58">
+        <v>4</v>
+      </c>
+      <c r="D58">
+        <f>D57/B58*A58/B58</f>
+        <v>965.625</v>
+      </c>
+      <c r="E58" s="2">
+        <f>D58/60</f>
+        <v>16.09375</v>
       </c>
     </row>
   </sheetData>
@@ -3453,6 +4024,7 @@
     <mergeCell ref="F28:H28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>